<commit_message>
Spreadsheet with results of the storage overhead experiment
</commit_message>
<xml_diff>
--- a/tests/weather/experiments/exp-runtime.xlsx
+++ b/tests/weather/experiments/exp-runtime.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="25">
   <si>
     <t xml:space="preserve">now </t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>overhead</t>
+  </si>
+  <si>
+    <t>20s</t>
+  </si>
+  <si>
+    <t>now</t>
+  </si>
+  <si>
+    <t>Trying to reformat</t>
   </si>
 </sst>
 </file>
@@ -203,8 +212,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -286,7 +299,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -317,6 +330,8 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -347,6 +362,8 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -371,8 +388,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -388,6 +406,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>summary!$B$2:$D$2</c:f>
@@ -423,7 +442,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -439,6 +457,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>summary!$B$2:$D$2</c:f>
@@ -474,7 +493,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -484,13 +502,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="2133049992"/>
-        <c:axId val="2133045384"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="2099632088"/>
+        <c:axId val="2099633688"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="2133049992"/>
+        <c:axId val="2099632088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -499,7 +517,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133045384"/>
+        <c:crossAx val="2099633688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -507,18 +525,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2133045384"/>
+        <c:axId val="2099633688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133049992"/>
+        <c:crossAx val="2099632088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -566,6 +603,418 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>summary!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>script</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>summary!$B$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>standalone</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>now </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>now with module bypass</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$B$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>20.22778579923333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.45155453683333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.45524517695556</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>overhead</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>summary!$B$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>standalone</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>now </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>now with module bypass</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$B$9:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.350658645211116</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.37211212983333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.596199267488885</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="2113158616"/>
+        <c:axId val="2109652760"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2113158616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2109652760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2109652760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2113158616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>script</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>summary!$B$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>standalone</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>now </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>now with module bypass</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$B$13:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>200.2762823634445</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200.4787822564444</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200.4833958677778</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>overhead</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>summary!$B$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>standalone</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>now </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>now with module bypass</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary!$B$14:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.36038430322219</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.46288441022227</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.584604132222182</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="2113075640"/>
+        <c:axId val="2113747864"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2113075640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2113747864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2113747864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2113075640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>now!$B$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -709,11 +1158,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2132967592"/>
-        <c:axId val="2132964504"/>
+        <c:axId val="2111076040"/>
+        <c:axId val="2108759176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2132967592"/>
+        <c:axId val="2111076040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -723,7 +1172,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132964504"/>
+        <c:crossAx val="2108759176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -731,7 +1180,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132964504"/>
+        <c:axId val="2108759176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -742,13 +1191,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132967592"/>
+        <c:crossAx val="2111076040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -768,15 +1218,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -790,6 +1240,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1155,14 +1669,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1218,9 +1733,167 @@
         <v>1.5885736700699997</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <f>standalone!M7</f>
+        <v>20.227785799233331</v>
+      </c>
+      <c r="C8" s="1">
+        <f>now!M14</f>
+        <v>20.451554536833331</v>
+      </c>
+      <c r="D8" s="1">
+        <f>'now with bypass'!M15</f>
+        <v>20.455245176955557</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <f>standalone!M8-B8</f>
+        <v>0.35065864521111578</v>
+      </c>
+      <c r="C9" s="1">
+        <f>now!M16-C8</f>
+        <v>16.372112129833329</v>
+      </c>
+      <c r="D9" s="1">
+        <f>'now with bypass'!M17-D8</f>
+        <v>1.5961992674888847</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <f>standalone!M9</f>
+        <v>200.27628236344447</v>
+      </c>
+      <c r="C13" s="1">
+        <f>now!M20</f>
+        <v>200.47878225644445</v>
+      </c>
+      <c r="D13" s="1">
+        <f>'now with bypass'!M21</f>
+        <v>200.4833958677778</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1">
+        <f>standalone!M10-B13</f>
+        <v>0.36038430322219028</v>
+      </c>
+      <c r="C14" s="1">
+        <f>now!M22-C13</f>
+        <v>16.462884410222273</v>
+      </c>
+      <c r="D14" s="1">
+        <f>'now with bypass'!M23-D13</f>
+        <v>1.5846041322221822</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f>B3</f>
+        <v>2.2264293299788891</v>
+      </c>
+      <c r="C20">
+        <f>B4</f>
+        <v>0.34779289224333354</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <f>C3</f>
+        <v>2.4276888900322224</v>
+      </c>
+      <c r="C21">
+        <f>C4</f>
+        <v>16.364755554412223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <f>D3</f>
+        <v>2.4388707743744451</v>
+      </c>
+      <c r="C22">
+        <f>D4</f>
+        <v>1.5885736700699997</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1238,7 +1911,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1590,8 +2263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updates on the execution time spreadsheet
</commit_message>
<xml_diff>
--- a/tests/weather/experiments/exp-runtime.xlsx
+++ b/tests/weather/experiments/exp-runtime.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1260" yWindow="0" windowWidth="49880" windowHeight="26600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="23">
   <si>
     <t xml:space="preserve">now </t>
   </si>
@@ -66,15 +66,6 @@
     <t>execution</t>
   </si>
   <si>
-    <t>Def</t>
-  </si>
-  <si>
-    <t>Dep</t>
-  </si>
-  <si>
-    <t>Exec</t>
-  </si>
-  <si>
     <t xml:space="preserve">time now run -b simulation.py data1.dat data2.dat </t>
   </si>
   <si>
@@ -93,10 +84,13 @@
     <t>20s</t>
   </si>
   <si>
-    <t>now</t>
+    <t>noWorkflow</t>
   </si>
   <si>
-    <t>Trying to reformat</t>
+    <t>noWorkflow with module bypass</t>
+  </si>
+  <si>
+    <t>200s</t>
   </si>
 </sst>
 </file>
@@ -112,6 +106,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -212,7 +207,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -278,8 +273,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -298,8 +295,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -332,6 +330,7 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -364,6 +363,7 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,6 +385,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>2 seconds</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -416,10 +435,10 @@
                   <c:v>standalone</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>now </c:v>
+                  <c:v>noWorkflow</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>now with module bypass</c:v>
+                  <c:v>noWorkflow with module bypass</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -467,10 +486,10 @@
                   <c:v>standalone</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>now </c:v>
+                  <c:v>noWorkflow</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>now with module bypass</c:v>
+                  <c:v>noWorkflow with module bypass</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -504,11 +523,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2099632088"/>
-        <c:axId val="2099633688"/>
+        <c:axId val="2088339832"/>
+        <c:axId val="2088343128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099632088"/>
+        <c:axId val="2088339832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -517,7 +536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099633688"/>
+        <c:crossAx val="2088343128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -525,9 +544,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099633688"/>
+        <c:axId val="2088343128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="250.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -555,9 +575,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099632088"/>
+        <c:crossAx val="2088339832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="25.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -591,6 +612,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>20 seconds</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -622,10 +662,10 @@
                   <c:v>standalone</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>now </c:v>
+                  <c:v>noWorkflow</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>now with module bypass</c:v>
+                  <c:v>noWorkflow with module bypass</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -673,10 +713,10 @@
                   <c:v>standalone</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>now </c:v>
+                  <c:v>noWorkflow</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>now with module bypass</c:v>
+                  <c:v>noWorkflow with module bypass</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -710,11 +750,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2113158616"/>
-        <c:axId val="2109652760"/>
+        <c:axId val="2088406920"/>
+        <c:axId val="2088409896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2113158616"/>
+        <c:axId val="2088406920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -723,7 +763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109652760"/>
+        <c:crossAx val="2088409896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -731,9 +771,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109652760"/>
+        <c:axId val="2088409896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="250.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -761,9 +802,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113158616"/>
+        <c:crossAx val="2088406920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="25.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -797,6 +839,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>200 seconds</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -828,10 +889,10 @@
                   <c:v>standalone</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>now </c:v>
+                  <c:v>noWorkflow</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>now with module bypass</c:v>
+                  <c:v>noWorkflow with module bypass</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -879,10 +940,10 @@
                   <c:v>standalone</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>now </c:v>
+                  <c:v>noWorkflow</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>now with module bypass</c:v>
+                  <c:v>noWorkflow with module bypass</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -916,11 +977,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2113075640"/>
-        <c:axId val="2113747864"/>
+        <c:axId val="2088439800"/>
+        <c:axId val="2088442776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2113075640"/>
+        <c:axId val="2088439800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -929,7 +990,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113747864"/>
+        <c:crossAx val="2088442776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -937,9 +998,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113747864"/>
+        <c:axId val="2088442776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -967,9 +1029,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113075640"/>
+        <c:crossAx val="2088439800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="25.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1015,42 +1078,24 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>now!$B$23</c:f>
+              <c:f>summary!$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Def</c:v>
+                  <c:v>definition</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>now!$C$22:$D$22</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.0000</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>220.968</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>216.924</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>now!$C$23:$D$23</c:f>
+              <c:f>summary!$B$20</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>0.0148315164778</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1061,42 +1106,24 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>now!$B$24</c:f>
+              <c:f>summary!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Dep</c:v>
+                  <c:v>deployment (environment)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>now!$C$22:$D$22</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.0000</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>220.968</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>216.924</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>now!$C$24:$D$24</c:f>
+              <c:f>summary!$B$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>0.0120259920756</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1107,50 +1134,61 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>now!$B$25</c:f>
+              <c:f>summary!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Exec</c:v>
+                  <c:v>deployment (modules)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>now!$C$22:$D$22</c:f>
+              <c:f>summary!$B$22</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.0000</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>220.968</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>216.924</c:v>
+                  <c:v>15.10577567417778</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>summary!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>execution</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>now!$C$25:$D$25</c:f>
+              <c:f>summary!$B$23</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>1.044894483444438</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1158,21 +1196,20 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2111076040"/>
-        <c:axId val="2108759176"/>
+        <c:axId val="2123062952"/>
+        <c:axId val="2118905688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2111076040"/>
+        <c:axId val="2123062952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="#,##0.0000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108759176"/>
+        <c:crossAx val="2118905688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1180,20 +1217,23 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108759176"/>
+        <c:axId val="2118905688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="18.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111076040"/>
+        <c:crossAx val="2123062952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0"/>
+        <c:minorUnit val="0.1"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1218,13 +1258,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:colOff>673100</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
@@ -1279,16 +1319,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1309,27 +1349,22 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1338,7 +1373,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1669,34 +1704,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B20" sqref="B20:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1718,7 +1754,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
         <f>standalone!M6-B3</f>
@@ -1735,14 +1771,14 @@
     </row>
     <row r="6" spans="1:4">
       <c r="B6" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
@@ -1770,7 +1806,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1">
         <f>standalone!M8-B8</f>
@@ -1787,14 +1823,14 @@
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>0</v>
@@ -1822,7 +1858,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1">
         <f>standalone!M10-B13</f>
@@ -1837,56 +1873,45 @@
         <v>1.5846041322221822</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <f>B3</f>
-        <v>2.2264293299788891</v>
-      </c>
-      <c r="C20">
-        <f>B4</f>
-        <v>0.34779289224333354</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21">
-        <f>C3</f>
-        <v>2.4276888900322224</v>
-      </c>
-      <c r="C21">
-        <f>C4</f>
-        <v>16.364755554412223</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <f>D3</f>
-        <v>2.4388707743744451</v>
-      </c>
-      <c r="C22">
-        <f>D4</f>
-        <v>1.5885736700699997</v>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="10">
+        <f>now!M17</f>
+        <v>1.4831516477800002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="10">
+        <f>now!M18</f>
+        <v>1.2025992075600001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="10">
+        <f>now!M19</f>
+        <v>15.105775674177778</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="10">
+        <f>now!M21-now!M20</f>
+        <v>1.0448944834444376</v>
       </c>
     </row>
   </sheetData>
@@ -2261,10 +2286,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3101,46 +3126,12 @@
         <v>216.94166666666672</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="B25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-      <c r="D25">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C3:L3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3169,12 +3160,12 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:13">

</xml_diff>

<commit_message>
Calculating the percentage of the module finder overhead
</commit_message>
<xml_diff>
--- a/tests/weather/experiments/exp-runtime.xlsx
+++ b/tests/weather/experiments/exp-runtime.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="0" windowWidth="49880" windowHeight="26600" tabRatio="500"/>
+    <workbookView xWindow="1260" yWindow="0" windowWidth="49880" windowHeight="26600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -283,6 +283,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -295,7 +296,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -523,11 +523,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2088339832"/>
-        <c:axId val="2088343128"/>
+        <c:axId val="2122716264"/>
+        <c:axId val="2122714120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2088339832"/>
+        <c:axId val="2122716264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -536,7 +536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088343128"/>
+        <c:crossAx val="2122714120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -544,7 +544,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2088343128"/>
+        <c:axId val="2122714120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250.0"/>
@@ -575,7 +575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088339832"/>
+        <c:crossAx val="2122716264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25.0"/>
@@ -750,11 +750,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2088406920"/>
-        <c:axId val="2088409896"/>
+        <c:axId val="2111713592"/>
+        <c:axId val="2111716568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2088406920"/>
+        <c:axId val="2111713592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -763,7 +763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088409896"/>
+        <c:crossAx val="2111716568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -771,7 +771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2088409896"/>
+        <c:axId val="2111716568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250.0"/>
@@ -802,7 +802,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088406920"/>
+        <c:crossAx val="2111713592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25.0"/>
@@ -977,11 +977,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2088439800"/>
-        <c:axId val="2088442776"/>
+        <c:axId val="2111749304"/>
+        <c:axId val="2111752280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2088439800"/>
+        <c:axId val="2111749304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -990,7 +990,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088442776"/>
+        <c:crossAx val="2111752280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -998,7 +998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2088442776"/>
+        <c:axId val="2111752280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1029,7 +1029,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088439800"/>
+        <c:crossAx val="2111749304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25.0"/>
@@ -1196,11 +1196,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2123062952"/>
-        <c:axId val="2118905688"/>
+        <c:axId val="2111798168"/>
+        <c:axId val="2111801144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2123062952"/>
+        <c:axId val="2111798168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1209,7 +1209,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118905688"/>
+        <c:crossAx val="2111801144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1217,7 +1217,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118905688"/>
+        <c:axId val="2111801144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -1229,7 +1229,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123062952"/>
+        <c:crossAx val="2111798168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1706,8 +1706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1718,11 +1718,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
@@ -1770,11 +1770,11 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" s="1" t="s">
@@ -1822,11 +1822,11 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="1" t="s">
@@ -1882,7 +1882,7 @@
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="6">
         <f>now!M17</f>
         <v>1.4831516477800002E-2</v>
       </c>
@@ -1891,7 +1891,7 @@
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="6">
         <f>now!M18</f>
         <v>1.2025992075600001E-2</v>
       </c>
@@ -1900,7 +1900,7 @@
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="6">
         <f>now!M19</f>
         <v>15.105775674177778</v>
       </c>
@@ -1909,7 +1909,7 @@
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="6">
         <f>now!M21-now!M20</f>
         <v>1.0448944834444376</v>
       </c>
@@ -1935,7 +1935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -1956,18 +1956,18 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
@@ -2286,10 +2286,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2297,31 +2297,31 @@
     <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="C3" s="7" t="s">
+    <row r="3" spans="1:14">
+      <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="9"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="10"/>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>1.3163752026044447E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>1.2100564108966668E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -2485,8 +2485,12 @@
         <f t="shared" si="0"/>
         <v>15.095867580833335</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7">
+        <f>(M7*100)/(M10-M8)</f>
+        <v>92.246214925973803</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -2528,7 +2532,7 @@
         <v>2.4276888900322224</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -2570,7 +2574,7 @@
         <v>3.3865282535555554</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -2612,7 +2616,7 @@
         <v>18.792444444444445</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>20</v>
       </c>
@@ -2654,7 +2658,7 @@
         <v>1.3308472103533333E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>20</v>
       </c>
@@ -2696,7 +2700,7 @@
         <v>1.1408408482888889E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>20</v>
       </c>
@@ -2738,7 +2742,7 @@
         <v>15.094477256155557</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>20</v>
       </c>
@@ -2780,7 +2784,7 @@
         <v>20.451554536833331</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14">
       <c r="A15" s="1">
         <v>20</v>
       </c>
@@ -2822,7 +2826,7 @@
         <v>21.419403367566666</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:14">
       <c r="A16" s="1">
         <v>20</v>
       </c>
@@ -3169,18 +3173,18 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">

</xml_diff>